<commit_message>
Coloquei mais dados na nossa base
</commit_message>
<xml_diff>
--- a/ManchetesRelevantes.xlsx
+++ b/ManchetesRelevantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Metricis\GoogleAlerts\EmailMetricis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235D64C4-26C4-4FE1-88D1-47225AAB090E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C800AF-0A24-4C11-B4E5-24E5CDE8B2D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D0F9D3E4-147D-44AE-BE13-A5F862DF1A29}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="295">
   <si>
     <t>Manchetes da Base de Dados</t>
   </si>
@@ -904,13 +904,31 @@
   </si>
   <si>
     <t>Beccar Varela advises on the launch of the first Social Impact Bond in Argentina</t>
+  </si>
+  <si>
+    <t>Social impact database</t>
+  </si>
+  <si>
+    <t>Pandemic Spurs Investor Interest in Social Bonds</t>
+  </si>
+  <si>
+    <t>Behavioral Health: A Payer-Based Strategy For Improving Access And Quality During COVID-19 And Beyond</t>
+  </si>
+  <si>
+    <t>Bonds deliver $562m boost to build social housing for vulnerable Australians</t>
+  </si>
+  <si>
+    <t>Blended finance for a Post-COVID19 world</t>
+  </si>
+  <si>
+    <t>Performance Based Contracting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -934,45 +952,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1003,42 +989,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1354,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28C7CE7-E55D-44AC-9D62-77518A654C25}">
-  <dimension ref="A1:C290"/>
+  <dimension ref="A1:C296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="A274" sqref="A274"/>
+    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,10 +1325,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1379,1923 +1336,1923 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="18">
+      <c r="B32" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B33" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="18">
+      <c r="B36" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="18">
+      <c r="B38" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="18">
+      <c r="B46" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B47" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18">
+      <c r="B48" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18">
+      <c r="B49" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18">
+      <c r="B50" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18">
+      <c r="B51" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18">
+      <c r="B52" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B53" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="18">
+      <c r="B54" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="18">
+      <c r="B55" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="18">
+      <c r="B56" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B57" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="18">
+      <c r="B58" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="18">
+      <c r="B59" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="18">
+      <c r="B60" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="18">
+      <c r="B61" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="18">
+      <c r="B62" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="18">
+      <c r="B63" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="18">
+      <c r="B64" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="18">
+      <c r="B65" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="18">
+      <c r="B66" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="18">
+      <c r="B67" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="18">
+      <c r="B68" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="18">
+      <c r="B69" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="18">
+      <c r="B70" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="18">
+      <c r="B71" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="18">
+      <c r="B72" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="18">
+      <c r="B73" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B74" s="18">
+      <c r="B74" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B75" s="18">
+      <c r="B75" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B76" s="18">
+      <c r="B76" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B77" s="18">
+      <c r="B77" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="18">
+      <c r="B78" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="18">
+      <c r="B79" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="18">
+      <c r="B80" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="18">
+      <c r="B81" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="18">
+      <c r="B82" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="18">
+      <c r="B83" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B84" s="18">
+      <c r="B84" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B85" s="18">
+      <c r="B85" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B86" s="18">
+      <c r="B86" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B87" s="18">
+      <c r="B87" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="18">
+      <c r="B88" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B89" s="18">
+      <c r="B89" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="18">
+      <c r="B90" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="18">
+      <c r="B91" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="18">
+      <c r="B92" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="18">
+      <c r="B93" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B94" s="18">
+      <c r="B94" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B95" s="18">
+      <c r="B95" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B96" s="18">
+      <c r="B96" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="18">
+      <c r="B97" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B98" s="18">
+      <c r="B98" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="18">
+      <c r="B99" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B100" s="18">
+      <c r="B100" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B101" s="18">
+      <c r="B101" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B102" s="18">
+      <c r="B102" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B103" s="18">
+      <c r="B103" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
+      <c r="A104" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B104" s="18">
+      <c r="B104" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
+      <c r="A105" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B105" s="18">
+      <c r="B105" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B106" s="18">
+      <c r="B106" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
+      <c r="A107" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B107" s="18">
+      <c r="B107" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
+      <c r="A108" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B108" s="18">
+      <c r="B108" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
+      <c r="A109" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B109" s="18">
+      <c r="B109" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
+      <c r="A110" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B110" s="18">
+      <c r="B110" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
+      <c r="A111" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="18">
+      <c r="B111" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
+      <c r="A112" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B112" s="18">
+      <c r="B112" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="9" t="s">
+      <c r="A113" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B113" s="18">
+      <c r="B113" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="9" t="s">
+      <c r="A114" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B114" s="18">
+      <c r="B114" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="9" t="s">
+      <c r="A115" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B115" s="18">
+      <c r="B115" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="9" t="s">
+      <c r="A116" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B116" s="18">
+      <c r="B116" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
+      <c r="A117" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B117" s="18">
+      <c r="B117" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="9" t="s">
+      <c r="A118" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B118" s="18">
+      <c r="B118" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="9" t="s">
+      <c r="A119" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B119" s="18">
+      <c r="B119" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="9" t="s">
+      <c r="A120" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B120" s="18">
+      <c r="B120" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="9" t="s">
+      <c r="A121" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B121" s="18">
+      <c r="B121" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
+      <c r="A122" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B122" s="18">
+      <c r="B122" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="9" t="s">
+      <c r="A123" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B123" s="18">
+      <c r="B123" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="9" t="s">
+      <c r="A124" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B124" s="18">
+      <c r="B124" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="9" t="s">
+      <c r="A125" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B125" s="18">
+      <c r="B125" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="9" t="s">
+      <c r="A126" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B126" s="18">
+      <c r="B126" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="9" t="s">
+      <c r="A127" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B127" s="18">
+      <c r="B127" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="9" t="s">
+      <c r="A128" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B128" s="18">
+      <c r="B128" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="9" t="s">
+      <c r="A129" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B129" s="18">
+      <c r="B129" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="9" t="s">
+      <c r="A130" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B130" s="18">
+      <c r="B130" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="9" t="s">
+      <c r="A131" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B131" s="18">
+      <c r="B131" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="9" t="s">
+      <c r="A132" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B132" s="18">
+      <c r="B132" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="9" t="s">
+      <c r="A133" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B133" s="18">
+      <c r="B133" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="9" t="s">
+      <c r="A134" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B134" s="18">
+      <c r="B134" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="9" t="s">
+      <c r="A135" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B135" s="18">
+      <c r="B135" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="9" t="s">
+      <c r="A136" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B136" s="18">
+      <c r="B136" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="9" t="s">
+      <c r="A137" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B137" s="18">
+      <c r="B137" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="9" t="s">
+      <c r="A138" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B138" s="18">
+      <c r="B138" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="9" t="s">
+      <c r="A139" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B139" s="18">
+      <c r="B139" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="9" t="s">
+      <c r="A140" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B140" s="18">
+      <c r="B140" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="8" t="s">
+      <c r="A141" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B141" s="18">
+      <c r="B141" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="9" t="s">
+      <c r="A142" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B142" s="18">
+      <c r="B142" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="9" t="s">
+      <c r="A143" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B143" s="18">
+      <c r="B143" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="9" t="s">
+      <c r="A144" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B144" s="18">
+      <c r="B144" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="9" t="s">
+      <c r="A145" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B145" s="18">
+      <c r="B145" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="9" t="s">
+      <c r="A146" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B146" s="18">
+      <c r="B146" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="9" t="s">
+      <c r="A147" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B147" s="18">
+      <c r="B147" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="9" t="s">
+      <c r="A148" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B148" s="18">
+      <c r="B148" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="9" t="s">
+      <c r="A149" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B149" s="18">
+      <c r="B149" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="9" t="s">
+      <c r="A150" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B150" s="18">
+      <c r="B150" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="9" t="s">
+      <c r="A151" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B151" s="18">
+      <c r="B151" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="9" t="s">
+      <c r="A152" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B152" s="18">
+      <c r="B152" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="9" t="s">
+      <c r="A153" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B153" s="18">
+      <c r="B153" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="9" t="s">
+      <c r="A154" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B154" s="18">
+      <c r="B154" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="9" t="s">
+      <c r="A155" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B155" s="18">
+      <c r="B155" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="9" t="s">
+      <c r="A156" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B156" s="18">
+      <c r="B156" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="9" t="s">
+      <c r="A157" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B157" s="18">
+      <c r="B157" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="9" t="s">
+      <c r="A158" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B158" s="18">
+      <c r="B158" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="9" t="s">
+      <c r="A159" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B159" s="18">
+      <c r="B159" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="9" t="s">
+      <c r="A160" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B160" s="18">
+      <c r="B160" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="9" t="s">
+      <c r="A161" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B161" s="18">
+      <c r="B161" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B162" s="18">
+      <c r="B162" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B163" s="18">
+      <c r="B163" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B164" s="18">
+      <c r="B164" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B165" s="18">
+      <c r="B165" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B166" s="18">
+      <c r="B166" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B167" s="18">
+      <c r="B167" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B168" s="18">
+      <c r="B168" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="9" t="s">
+      <c r="A169" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B169" s="18">
+      <c r="B169" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" s="9" t="s">
+      <c r="A170" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B170" s="18">
+      <c r="B170" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="9" t="s">
+      <c r="A171" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B171" s="18">
+      <c r="B171" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="9" t="s">
+      <c r="A172" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B172" s="18">
+      <c r="B172" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="9" t="s">
+      <c r="A173" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B173" s="18">
+      <c r="B173" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="9" t="s">
+      <c r="A174" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B174" s="18">
+      <c r="B174" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="9" t="s">
+      <c r="A175" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B175" s="18">
+      <c r="B175" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" s="9" t="s">
+      <c r="A176" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B176" s="18">
+      <c r="B176" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="9" t="s">
+      <c r="A177" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B177" s="18">
+      <c r="B177" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="9" t="s">
+      <c r="A178" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B178" s="18">
+      <c r="B178" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="3" t="s">
+      <c r="A179" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B179" s="18">
+      <c r="B179" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" s="3" t="s">
+      <c r="A180" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B180" s="18">
+      <c r="B180" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B181" s="18">
+      <c r="B181" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B182" s="18">
+      <c r="B182" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="A183" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B183" s="18">
+      <c r="B183" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
+      <c r="A184" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B184" s="18">
+      <c r="B184" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B185" s="18">
+      <c r="B185" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B186" s="18">
+      <c r="B186" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="s">
+      <c r="A187" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B187" s="18">
+      <c r="B187" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="10" t="s">
+      <c r="A188" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B188" s="18">
+      <c r="B188" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="9" t="s">
+      <c r="A189" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B189" s="18">
+      <c r="B189" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="10" t="s">
+      <c r="A190" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B190" s="18">
+      <c r="B190" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="9" t="s">
+      <c r="A191" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B191" s="18">
+      <c r="B191" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" s="9" t="s">
+      <c r="A192" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B192" s="18">
+      <c r="B192" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="9" t="s">
+      <c r="A193" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B193" s="18">
+      <c r="B193" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="9" t="s">
+      <c r="A194" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B194" s="18">
+      <c r="B194" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="9" t="s">
+      <c r="A195" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B195" s="18">
+      <c r="B195" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="9" t="s">
+      <c r="A196" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B196" s="18">
+      <c r="B196" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="9" t="s">
+      <c r="A197" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B197" s="18">
+      <c r="B197" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="8" t="s">
+      <c r="A198" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B198" s="18">
+      <c r="B198" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="9" t="s">
+      <c r="A199" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B199" s="18">
+      <c r="B199" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A200" s="9" t="s">
+      <c r="A200" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B200" s="18">
+      <c r="B200" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A201" s="9" t="s">
+      <c r="A201" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B201" s="18">
+      <c r="B201" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A202" s="9" t="s">
+      <c r="A202" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B202" s="18">
+      <c r="B202" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A203" s="9" t="s">
+      <c r="A203" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B203" s="18">
+      <c r="B203" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="9" t="s">
+      <c r="A204" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B204" s="18">
+      <c r="B204" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="9" t="s">
+      <c r="A205" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B205" s="18">
+      <c r="B205" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A206" s="9" t="s">
+      <c r="A206" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B206" s="18">
+      <c r="B206" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="9" t="s">
+      <c r="A207" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B207" s="18">
+      <c r="B207" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A208" s="9" t="s">
+      <c r="A208" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B208" s="18">
+      <c r="B208" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="9" t="s">
+      <c r="A209" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B209" s="18">
+      <c r="B209" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="9" t="s">
+      <c r="A210" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="B210" s="18">
+      <c r="B210" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="8" t="s">
+      <c r="A211" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B211" s="18">
+      <c r="B211" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="11" t="s">
+      <c r="A212" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B212" s="18">
+      <c r="B212" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="3" t="s">
+      <c r="A213" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B213" s="18">
+      <c r="B213" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="3" t="s">
+      <c r="A214" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B214" s="18">
+      <c r="B214" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="3" t="s">
+      <c r="A215" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B215" s="18">
+      <c r="B215" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
+      <c r="A216" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B216" s="18">
+      <c r="B216" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" s="3" t="s">
+      <c r="A217" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="B217" s="18">
+      <c r="B217" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="3" t="s">
+      <c r="A218" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="B218" s="18">
+      <c r="B218" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" s="3" t="s">
+      <c r="A219" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B219" s="18">
+      <c r="B219" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" s="3" t="s">
+      <c r="A220" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B220" s="18">
+      <c r="B220" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" s="9" t="s">
+      <c r="A221" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B221" s="18">
+      <c r="B221" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="9" t="s">
+      <c r="A222" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B222" s="18">
+      <c r="B222" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" s="9" t="s">
+      <c r="A223" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B223" s="18">
+      <c r="B223" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="10" t="s">
+      <c r="A224" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B224" s="18">
+      <c r="B224" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A225" s="9" t="s">
+      <c r="A225" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B225" s="18">
+      <c r="B225" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="12" t="s">
+      <c r="A226" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B226" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A227" s="13" t="s">
+      <c r="B226" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B227" s="18">
+      <c r="B227" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A228" s="9" t="s">
+      <c r="A228" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B228" s="18">
+      <c r="B228" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="9" t="s">
+      <c r="A229" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B229" s="18">
+      <c r="B229" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="9" t="s">
+      <c r="A230" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B230" s="18">
+      <c r="B230" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A231" s="9" t="s">
+      <c r="A231" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B231" s="18">
+      <c r="B231" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="9" t="s">
+      <c r="A232" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B232" s="18">
+      <c r="B232" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="9" t="s">
+      <c r="A233" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B233" s="18">
+      <c r="B233" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A234" s="9" t="s">
+      <c r="A234" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B234" s="18">
+      <c r="B234" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A235" s="9" t="s">
+      <c r="A235" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B235" s="18">
+      <c r="B235" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="9" t="s">
+      <c r="A236" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B236" s="18">
+      <c r="B236" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="9" t="s">
+      <c r="A237" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B237" s="18">
+      <c r="B237" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="9" t="s">
+      <c r="A238" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B238" s="18">
+      <c r="B238" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="9" t="s">
+      <c r="A239" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B239" s="18">
+      <c r="B239" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="9" t="s">
+      <c r="A240" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B240" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A241" s="14" t="s">
+      <c r="B240" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B241" s="18">
+      <c r="B241" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3303,7 +3260,7 @@
       <c r="A242" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B242" s="18">
+      <c r="B242" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3311,7 +3268,7 @@
       <c r="A243" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B243" s="18">
+      <c r="B243" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3319,7 +3276,7 @@
       <c r="A244" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B244" s="18">
+      <c r="B244" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3327,15 +3284,15 @@
       <c r="A245" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B245" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B245" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B246" s="18">
+      <c r="B246" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3343,39 +3300,39 @@
       <c r="A247" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B247" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A248" s="15" t="s">
+      <c r="B247" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B248" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B248" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B249" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B249" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="B250" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B250" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="B251" s="18">
+      <c r="B251" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3383,7 +3340,7 @@
       <c r="A252" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B252" s="18">
+      <c r="B252" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3391,7 +3348,7 @@
       <c r="A253" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B253" s="18">
+      <c r="B253" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3399,23 +3356,23 @@
       <c r="A254" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="B254" s="18">
+      <c r="B254" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="16" t="s">
+      <c r="A255" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="B255" s="18">
+      <c r="B255" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="15" t="s">
+      <c r="A256" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="B256" s="18">
+      <c r="B256" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3423,7 +3380,7 @@
       <c r="A257" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B257" s="18">
+      <c r="B257" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3431,7 +3388,7 @@
       <c r="A258" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B258" s="18">
+      <c r="B258" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3439,7 +3396,7 @@
       <c r="A259" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B259" s="18">
+      <c r="B259" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3447,7 +3404,7 @@
       <c r="A260" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B260" s="18">
+      <c r="B260" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3455,7 +3412,7 @@
       <c r="A261" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="B261" s="18">
+      <c r="B261" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3463,7 +3420,7 @@
       <c r="A262" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B262" s="18">
+      <c r="B262" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3471,7 +3428,7 @@
       <c r="A263" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B263" s="18">
+      <c r="B263" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3479,7 +3436,7 @@
       <c r="A264" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="B264" s="18">
+      <c r="B264" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3487,7 +3444,7 @@
       <c r="A265" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B265" s="18">
+      <c r="B265" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3495,7 +3452,7 @@
       <c r="A266" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B266" s="18">
+      <c r="B266" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3503,7 +3460,7 @@
       <c r="A267" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B267" s="18">
+      <c r="B267" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3511,7 +3468,7 @@
       <c r="A268" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B268" s="18">
+      <c r="B268" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3519,15 +3476,15 @@
       <c r="A269" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B269" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B269" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B270" s="18">
+      <c r="B270" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3535,7 +3492,7 @@
       <c r="A271" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B271" s="18">
+      <c r="B271" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3543,151 +3500,199 @@
       <c r="A272" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B272" s="18">
+      <c r="B272" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="6" t="s">
+      <c r="A273" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B273" s="18">
+      <c r="B273" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="6" t="s">
+      <c r="A274" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B274" s="18">
+      <c r="B274" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="6" t="s">
+      <c r="A275" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B275" s="18">
+      <c r="B275" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="6" t="s">
+      <c r="A276" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="B276" s="18">
+      <c r="B276" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="17" t="s">
+      <c r="A277" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B277" s="18">
+      <c r="B277" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="18" t="s">
+      <c r="A278" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B278" s="18">
+      <c r="B278" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="18" t="s">
+      <c r="A279" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B279" s="18">
+      <c r="B279" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="17" t="s">
+      <c r="A280" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B280" s="18">
+      <c r="B280" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="18" t="s">
+      <c r="A281" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B281" s="18">
+      <c r="B281" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="18" t="s">
+      <c r="A282" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B282" s="18">
+      <c r="B282" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="18" t="s">
+      <c r="A283" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B283" s="18">
+      <c r="B283" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="18" t="s">
+      <c r="A284" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B284" s="18">
+      <c r="B284" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="18" t="s">
+      <c r="A285" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B285" s="18">
+      <c r="B285" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="18" t="s">
+      <c r="A286" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B286" s="18">
+      <c r="B286" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="18" t="s">
+      <c r="A287" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B287" s="18">
+      <c r="B287" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="18" t="s">
+      <c r="A288" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B288" s="18">
+      <c r="B288" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="18" t="s">
+      <c r="A289" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B289" s="18">
+      <c r="B289" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="18" t="s">
+      <c r="A290" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B290" s="18">
+      <c r="B290" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B291" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B292" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B293" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B294" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B295" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B296" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3698,9 +3703,10 @@
     <hyperlink ref="A248" r:id="rId3" display="https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://weetracker.com/2020/04/04/afdb-usd-3-bn-social-bond-listed-london-stock-exchange/&amp;ct=ga&amp;cd=CAEYACoUMTQyMTUzMjc4NTEwNzk3Njk2MzIyHWFjZjEzZjhjNThkNjYxZDk6Y29tLmJyOmVuOkJS&amp;usg=AFQjCNFwwDhHVJ45nE4NYOtMvCn1YSqzJQ" xr:uid="{31A03655-F385-4440-AB4D-369276F54ED4}"/>
     <hyperlink ref="A255" r:id="rId4" display="https://www.semanticscholar.org/paper/520ea106e8539029639d5ad44022bbfcf3a33b4f?p2df" xr:uid="{32D4ACFE-2502-4C04-9436-152A30D3BAC7}"/>
     <hyperlink ref="A256" r:id="rId5" display="https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://www.thenational.ae/business/money/how-to-donate-to-uae-charities-helping-those-affected-by-covid-19-1.1002315&amp;ct=ga&amp;cd=CAEYASoTODk5OTU5NTg4NDQyNTkyMzI4ODIdYWNmMTNmOGM1OGQ2NjFkOTpjb20uYnI6ZW46QlI&amp;usg=AFQjCNE8DXVvKMic9jVNfz1K3mjX5Ygu-Q" xr:uid="{BC0A2041-5B30-4923-8B6D-34C84C5E2041}"/>
+    <hyperlink ref="A291" r:id="rId6" display="https://www.google.com/url?rct=j&amp;sa=t&amp;url=https://bocafriendshiphouse.com/opwmwda/social-impact-database.html&amp;ct=ga&amp;cd=CAEYACoUMTM1MzY0MjEwNDU1MzY2NTAzNzMyHWFjZjEzZjhjNThkNjYxZDk6Y29tLmJyOmVuOkJS&amp;usg=AFQjCNFTJkdjimKZVe-EeKxexQyEdTch1A" xr:uid="{E708AA31-8110-4614-8E16-1341ADF713C3}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>